<commit_message>
Refactor fetchers and CLI for improved functionality and debugging
- Updated `test_fetch_sudecap.py` to enhance error handling and add output directory option.
- Removed unused bytecode files from `__pycache__` directories.
- Refactored `cli.py` to comment out unused fetchers and prepare for future reactivation.
- Introduced helper functions for fetching and validating files in `sinapi.py` and `sudecap.py`.
- Enhanced logging for debugging HTTP requests in `http.py`, `sinapi.py`, and `sudecap.py`.
- Updated fetch logic to handle file existence checks and improved response handling.
- Added headers for requests to avoid HTML responses from servers.
</commit_message>
<xml_diff>
--- a/output/cruzamento_sinapi_2025_06.xlsx
+++ b/output/cruzamento_sinapi_2025_06.xlsx
@@ -544,7 +544,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Teste TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
+          <t>TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">
@@ -1060,7 +1060,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1069,10 +1069,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="26" customWidth="1" min="2" max="2"/>
+    <col width="9" customWidth="1" min="2" max="2"/>
     <col width="9" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
-    <col width="5" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1096,30 +1095,6 @@
           <t>dif_rel</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>dir</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>100251</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>['DESCRICAO_DIVERGENTE']</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>